<commit_message>
Bulk user registration with excel file and sample excel file download
</commit_message>
<xml_diff>
--- a/src/assets/bulkuser_excel_sheet.xlsx
+++ b/src/assets/bulkuser_excel_sheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19380" windowHeight="7360"/>
+    <workbookView windowWidth="19160" windowHeight="6350"/>
   </bookViews>
   <sheets>
     <sheet name="Bulk User" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="159">
   <si>
     <t>Title</t>
   </si>
@@ -64,7 +64,7 @@
     <t>EmergencyContactNo</t>
   </si>
   <si>
-    <t>DOB</t>
+    <t>DateOfBirth</t>
   </si>
   <si>
     <t>Age</t>
@@ -73,6 +73,12 @@
     <t>Email</t>
   </si>
   <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
     <t>MaritalStatus</t>
   </si>
   <si>
@@ -97,39 +103,42 @@
     <t>Religion</t>
   </si>
   <si>
-    <t>AddressLine1</t>
+    <t>CurrentAddressLine1</t>
+  </si>
+  <si>
+    <t>CurrentState</t>
+  </si>
+  <si>
+    <t>CurrentDistrict</t>
+  </si>
+  <si>
+    <t>CurrentPincode</t>
+  </si>
+  <si>
+    <t>PermanentAddressLine1</t>
+  </si>
+  <si>
+    <t>PermanentState</t>
+  </si>
+  <si>
+    <t>PermanentDistrict</t>
+  </si>
+  <si>
+    <t>PermanentPincode</t>
+  </si>
+  <si>
+    <t>DateOfJoining</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Marital Status</t>
   </si>
   <si>
     <t>State</t>
   </si>
   <si>
-    <t>District</t>
-  </si>
-  <si>
-    <t>Pincode</t>
-  </si>
-  <si>
-    <t>PermanentAddressLine1</t>
-  </si>
-  <si>
-    <t>PermanentState</t>
-  </si>
-  <si>
-    <t>PermanentDistrict</t>
-  </si>
-  <si>
-    <t>PermanentPincode</t>
-  </si>
-  <si>
-    <t>DateOfJoining</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Marital Status</t>
-  </si>
-  <si>
     <t>Male</t>
   </si>
   <si>
@@ -148,6 +157,9 @@
     <t>General</t>
   </si>
   <si>
+    <t>Hindu</t>
+  </si>
+  <si>
     <t>Andaman and Nicobar Islands</t>
   </si>
   <si>
@@ -167,6 +179,9 @@
   </si>
   <si>
     <t>SC</t>
+  </si>
+  <si>
+    <t>Muslim</t>
   </si>
   <si>
     <t>Andhra Pradesh</t>
@@ -194,6 +209,9 @@
     <t>ST</t>
   </si>
   <si>
+    <t>Christian</t>
+  </si>
+  <si>
     <t>Arunachal Pradesh</t>
   </si>
   <si>
@@ -215,6 +233,9 @@
     <t>BC</t>
   </si>
   <si>
+    <t>Sikh</t>
+  </si>
+  <si>
     <t>Assam</t>
   </si>
   <si>
@@ -233,6 +254,9 @@
     <t>OBC</t>
   </si>
   <si>
+    <t>Buddism</t>
+  </si>
+  <si>
     <t>Bihar</t>
   </si>
   <si>
@@ -248,6 +272,9 @@
     <t>OC</t>
   </si>
   <si>
+    <t>Jainism</t>
+  </si>
+  <si>
     <t>Chandigarh</t>
   </si>
   <si>
@@ -260,6 +287,9 @@
     <t>Not given</t>
   </si>
   <si>
+    <t>Other</t>
+  </si>
+  <si>
     <t>Chattisgarh</t>
   </si>
   <si>
@@ -269,10 +299,16 @@
     <t>Tea Tribe</t>
   </si>
   <si>
+    <t>Parsi</t>
+  </si>
+  <si>
     <t>Dadra and Nagar Haveli</t>
   </si>
   <si>
     <t>Dean Medical College</t>
+  </si>
+  <si>
+    <t>Not Disclosed</t>
   </si>
   <si>
     <t>Daman and Diu</t>
@@ -486,13 +522,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="[$-14009]yyyy/mm/dd;@"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -501,32 +538,53 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
+      <sz val="18"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -975,162 +1033,168 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1450,149 +1514,138 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AB6"/>
+  <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="8.21818181818182" customWidth="1"/>
-    <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="13.4454545454545" customWidth="1"/>
-    <col min="4" max="4" width="10.6636363636364" customWidth="1"/>
-    <col min="5" max="5" width="16.3363636363636" customWidth="1"/>
-    <col min="6" max="6" width="11.2181818181818" customWidth="1"/>
-    <col min="7" max="7" width="12" customWidth="1"/>
-    <col min="8" max="8" width="21.7818181818182" style="3" customWidth="1"/>
-    <col min="9" max="9" width="10.3363636363636" customWidth="1"/>
-    <col min="10" max="10" width="4.55454545454545" customWidth="1"/>
-    <col min="11" max="11" width="25.3363636363636" customWidth="1"/>
-    <col min="12" max="12" width="13.8909090909091" customWidth="1"/>
-    <col min="13" max="13" width="24.7818181818182" style="3" customWidth="1"/>
-    <col min="14" max="14" width="11.8909090909091" customWidth="1"/>
-    <col min="15" max="15" width="12.7818181818182" customWidth="1"/>
-    <col min="16" max="16" width="12.8909090909091" customWidth="1"/>
-    <col min="17" max="17" width="13.8909090909091" customWidth="1"/>
-    <col min="18" max="18" width="11.6636363636364" customWidth="1"/>
-    <col min="20" max="27" width="28.8909090909091" customWidth="1"/>
-    <col min="28" max="28" width="21.1090909090909" customWidth="1"/>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="23.1272727272727" customWidth="1"/>
+    <col min="4" max="4" width="20.7545454545455" customWidth="1"/>
+    <col min="5" max="5" width="17.1272727272727" customWidth="1"/>
+    <col min="6" max="6" width="22.5" style="4" customWidth="1"/>
+    <col min="7" max="7" width="19.3727272727273" customWidth="1"/>
+    <col min="8" max="8" width="32.2545454545455" style="4" customWidth="1"/>
+    <col min="9" max="9" width="21.1272727272727" style="5" customWidth="1"/>
+    <col min="10" max="10" width="9.12727272727273" style="4" customWidth="1"/>
+    <col min="11" max="13" width="25.3727272727273" customWidth="1"/>
+    <col min="14" max="14" width="24" customWidth="1"/>
+    <col min="15" max="15" width="24.7545454545455" style="4" customWidth="1"/>
+    <col min="16" max="16" width="11.8727272727273" customWidth="1"/>
+    <col min="17" max="17" width="20.6272727272727" customWidth="1"/>
+    <col min="18" max="18" width="20.1272727272727" customWidth="1"/>
+    <col min="19" max="19" width="20.7545454545455" customWidth="1"/>
+    <col min="20" max="20" width="20.3727272727273" customWidth="1"/>
+    <col min="21" max="21" width="16.7545454545455" customWidth="1"/>
+    <col min="22" max="24" width="28.8727272727273" customWidth="1"/>
+    <col min="25" max="25" width="21.6272727272727" style="4" customWidth="1"/>
+    <col min="26" max="26" width="35.6272727272727" customWidth="1"/>
+    <col min="27" max="28" width="28.8727272727273" customWidth="1"/>
+    <col min="29" max="29" width="28.8727272727273" style="4" customWidth="1"/>
+    <col min="30" max="30" width="21.1272727272727" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28">
-      <c r="A1" s="4" t="s">
+    <row r="1" s="3" customFormat="1" ht="23.5" spans="1:30">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="U1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="V1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="W1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="X1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Y1" s="11" t="s">
         <v>24</v>
       </c>
       <c r="Z1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AA1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AB1" s="13" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="6:13">
-      <c r="F2" s="6"/>
-      <c r="H2"/>
-      <c r="M2"/>
-    </row>
-    <row r="3" spans="6:13">
-      <c r="F3" s="6"/>
-      <c r="H3"/>
-      <c r="M3"/>
-    </row>
-    <row r="4" spans="6:13">
-      <c r="F4" s="6"/>
-      <c r="H4"/>
-      <c r="M4"/>
-    </row>
-    <row r="5" spans="6:13">
-      <c r="F5" s="6"/>
-      <c r="H5"/>
-      <c r="M5"/>
-    </row>
-    <row r="6" spans="6:13">
-      <c r="F6" s="6"/>
-      <c r="H6"/>
-      <c r="M6"/>
+      <c r="AC1" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="11:11">
+      <c r="K2" s="12"/>
     </row>
   </sheetData>
-  <dataValidations count="9">
+  <dataValidations count="8">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576">
       <formula1>Help!$C$2:$C$7</formula1>
     </dataValidation>
@@ -1602,31 +1655,25 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576">
       <formula1>Help!$D$2:$D$50</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N1048576">
       <formula1>Help!$E$2:$E$8</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q1048576">
       <formula1>Help!$F$2:$F$6</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R$1:R$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T$1:T$1048576">
       <formula1>Help!$G$2:$G$9</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:S1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:U1048576">
       <formula1>Help!$H$2:$H$9</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:U1048576 Y2:Y1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W2:W1048576 AA2:AA1048576">
       <formula1>Help!$I$2:$I$38</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z7:Z1048576 C3:D6">
-      <formula1>Help!$I:$I</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>
   <headerFooter/>
-  <ignoredErrors>
-    <ignoredError sqref="R1" listDataValidation="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -1636,26 +1683,26 @@
   <dimension ref="A1:I50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I$1:I$1048576"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="17.4454545454545" customWidth="1"/>
-    <col min="2" max="2" width="16.1090909090909" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.89090909090909" style="1"/>
-    <col min="4" max="4" width="32.6636363636364" customWidth="1"/>
-    <col min="5" max="5" width="13.6636363636364" customWidth="1"/>
-    <col min="6" max="6" width="19.4454545454545" customWidth="1"/>
-    <col min="7" max="7" width="13.5545454545455" customWidth="1"/>
-    <col min="8" max="8" width="13.7818181818182" customWidth="1"/>
-    <col min="9" max="9" width="27.1090909090909" customWidth="1"/>
-    <col min="12" max="12" width="8.89090909090909" customWidth="1"/>
+    <col min="1" max="1" width="17.5" customWidth="1"/>
+    <col min="2" max="2" width="16.1272727272727" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.87272727272727" style="1"/>
+    <col min="4" max="4" width="32.6272727272727" customWidth="1"/>
+    <col min="5" max="5" width="13.6272727272727" customWidth="1"/>
+    <col min="6" max="6" width="19.5" customWidth="1"/>
+    <col min="7" max="7" width="13.5" customWidth="1"/>
+    <col min="8" max="8" width="13.7545454545455" customWidth="1"/>
+    <col min="9" max="9" width="27.1272727272727" customWidth="1"/>
+    <col min="12" max="12" width="8.87272727272727" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>4</v>
@@ -1667,19 +1714,19 @@
         <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -1687,28 +1734,28 @@
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G2" t="s">
-        <v>35</v>
-      </c>
-      <c r="H2" t="s">
-        <v>35</v>
+        <v>38</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="I2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1716,465 +1763,469 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E3" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F3" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="G3" t="s">
-        <v>42</v>
-      </c>
-      <c r="H3" t="s">
-        <v>42</v>
+        <v>46</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="I3" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" ht="15.6" customHeight="1" spans="1:9">
       <c r="A4" s="2" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D4" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E4" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="F4" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="G4" t="s">
-        <v>50</v>
-      </c>
-      <c r="H4" t="s">
-        <v>50</v>
+        <v>55</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="I4" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="E5" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="F5" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="G5" t="s">
-        <v>57</v>
-      </c>
-      <c r="H5" t="s">
-        <v>57</v>
+        <v>63</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="I5" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="D6" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="E6" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="F6" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="G6" t="s">
-        <v>63</v>
-      </c>
-      <c r="H6" t="s">
-        <v>63</v>
+        <v>70</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="I6" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="D7" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="E7" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="G7" t="s">
-        <v>68</v>
-      </c>
-      <c r="H7" t="s">
-        <v>68</v>
+        <v>76</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="I7" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="E8" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="G8" t="s">
-        <v>72</v>
-      </c>
-      <c r="H8" t="s">
-        <v>72</v>
+        <v>81</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="I8" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="4:9">
       <c r="D9" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="G9" t="s">
-        <v>75</v>
-      </c>
-      <c r="H9" t="s">
-        <v>75</v>
+        <v>85</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="I9" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="4:9">
       <c r="D10" t="s">
-        <v>77</v>
+        <v>88</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>89</v>
       </c>
       <c r="I10" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="4:9">
       <c r="D11" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="I11" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="4:9">
       <c r="D12" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="I12" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="4:9">
       <c r="D13" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="I13" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="4:9">
       <c r="D14" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="I14" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="4:9">
       <c r="D15" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="I15" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="4:9">
       <c r="D16" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="I16" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="4:9">
       <c r="D17" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="I17" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="4:9">
       <c r="D18" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="I18" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="4:9">
       <c r="D19" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="I19" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" spans="4:9">
       <c r="D20" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="I20" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21" spans="4:9">
       <c r="D21" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="I21" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="4:9">
       <c r="D22" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="I22" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" spans="4:9">
       <c r="D23" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="I23" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24" spans="4:9">
       <c r="D24" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="I24" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25" spans="4:9">
       <c r="D25" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="I25" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
     </row>
     <row r="26" spans="4:9">
       <c r="D26" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="I26" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
     </row>
     <row r="27" spans="4:9">
       <c r="D27" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="I27" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
     </row>
     <row r="28" spans="4:9">
       <c r="D28" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="I28" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
     </row>
     <row r="29" spans="4:9">
       <c r="D29" t="s">
-        <v>115</v>
+        <v>127</v>
       </c>
       <c r="I29" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
     </row>
     <row r="30" spans="4:9">
       <c r="D30" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="I30" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
     </row>
     <row r="31" spans="4:9">
       <c r="D31" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
       <c r="I31" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
     </row>
     <row r="32" spans="4:9">
       <c r="D32" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="I32" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
     </row>
     <row r="33" spans="4:9">
       <c r="D33" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="I33" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
     </row>
     <row r="34" spans="4:9">
       <c r="D34" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="I34" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
     </row>
     <row r="35" spans="4:9">
       <c r="D35" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="I35" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
     </row>
     <row r="36" spans="4:9">
       <c r="D36" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="I36" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
     </row>
     <row r="37" spans="4:9">
       <c r="D37" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
       <c r="I37" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
     </row>
     <row r="38" spans="4:9">
       <c r="D38" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="I38" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
     </row>
     <row r="39" spans="4:4">
       <c r="D39" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
     </row>
     <row r="40" spans="4:4">
       <c r="D40" t="s">
-        <v>136</v>
+        <v>148</v>
       </c>
     </row>
     <row r="41" spans="4:4">
       <c r="D41" t="s">
-        <v>137</v>
+        <v>149</v>
       </c>
     </row>
     <row r="42" spans="4:4">
       <c r="D42" t="s">
-        <v>138</v>
+        <v>150</v>
       </c>
     </row>
     <row r="43" spans="4:4">
       <c r="D43" t="s">
-        <v>139</v>
+        <v>151</v>
       </c>
     </row>
     <row r="44" spans="4:4">
       <c r="D44" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
     </row>
     <row r="45" spans="4:4">
       <c r="D45" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
     </row>
     <row r="46" spans="4:4">
       <c r="D46" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
     </row>
     <row r="47" spans="4:4">
       <c r="D47" t="s">
-        <v>143</v>
+        <v>155</v>
       </c>
     </row>
     <row r="48" spans="4:4">
       <c r="D48" t="s">
-        <v>144</v>
+        <v>156</v>
       </c>
     </row>
     <row r="49" spans="4:4">
       <c r="D49" t="s">
-        <v>145</v>
+        <v>157</v>
       </c>
     </row>
     <row r="50" spans="4:4">
       <c r="D50" t="s">
-        <v>146</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>